<commit_message>
Updated distance sorting and flow on
</commit_message>
<xml_diff>
--- a/Data/distanceTravelled.xlsx
+++ b/Data/distanceTravelled.xlsx
@@ -25,58 +25,58 @@
     <t>Distance</t>
   </si>
   <si>
+    <t>Carlton</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
     <t>Adelaide Crows</t>
   </si>
   <si>
-    <t>VIC</t>
+    <t>GWS Giants</t>
+  </si>
+  <si>
+    <t>Fremantle</t>
+  </si>
+  <si>
+    <t>Gold Coast Suns</t>
+  </si>
+  <si>
+    <t>Essendon</t>
+  </si>
+  <si>
+    <t>Collingwood</t>
   </si>
   <si>
     <t>Brisbane Lions</t>
   </si>
   <si>
-    <t>Carlton</t>
-  </si>
-  <si>
-    <t>Collingwood</t>
-  </si>
-  <si>
-    <t>Essendon</t>
-  </si>
-  <si>
-    <t>Fremantle</t>
-  </si>
-  <si>
-    <t>GWS Giants</t>
+    <t>Melbourne</t>
   </si>
   <si>
     <t>Geelong Cats</t>
   </si>
   <si>
-    <t>Gold Coast Suns</t>
-  </si>
-  <si>
     <t>Hawthorn</t>
   </si>
   <si>
-    <t>Melbourne</t>
+    <t>Port Adelaide</t>
   </si>
   <si>
     <t>North Melbourne</t>
   </si>
   <si>
-    <t>Port Adelaide</t>
+    <t>St Kilda</t>
   </si>
   <si>
     <t>Richmond</t>
   </si>
   <si>
-    <t>St Kilda</t>
+    <t>West Coast Eagles</t>
   </si>
   <si>
     <t>Sydney Swans</t>
-  </si>
-  <si>
-    <t>West Coast Eagles</t>
   </si>
   <si>
     <t>Western Bulldogs</t>

</xml_diff>